<commit_message>
updated git commands file
</commit_message>
<xml_diff>
--- a/Git Commands.xlsx
+++ b/Git Commands.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Command Syntax</t>
   </si>
@@ -147,16 +147,27 @@
   </si>
   <si>
     <t>To pull the changes from remote repository</t>
+  </si>
+  <si>
+    <t>https://rubygarage.org/blog/most-basic-git-commands-with-examples</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,13 +190,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,15 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="194.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -644,8 +658,16 @@
         <v>40</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A23" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified git commands file
</commit_message>
<xml_diff>
--- a/Git Commands.xlsx
+++ b/Git Commands.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Command Syntax</t>
   </si>
@@ -150,6 +150,24 @@
   </si>
   <si>
     <t>https://rubygarage.org/blog/most-basic-git-commands-with-examples</t>
+  </si>
+  <si>
+    <t>$ git commit -m 'message'</t>
+  </si>
+  <si>
+    <t>$ git commit</t>
+  </si>
+  <si>
+    <t>To commit your changes at local repository but this will open new editor window and you have to press 'I' to start typing and after typing message, type ':wq' to go back to git bash and to escape from new editor</t>
+  </si>
+  <si>
+    <t>To commit your changes at local repository(using this way you can skip edit stage)</t>
+  </si>
+  <si>
+    <t>$ clear</t>
+  </si>
+  <si>
+    <t>To clear the window</t>
   </si>
 </sst>
 </file>
@@ -478,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,14 +676,38 @@
         <v>40</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A23" r:id="rId1"/>
+    <hyperlink ref="A25" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>